<commit_message>
Resources: Update PP_PhmSoftPowerPlayTable config
</commit_message>
<xml_diff>
--- a/Resources/GPU/XFX RX5700 XT THICC II Ultra OC.xlsx
+++ b/Resources/GPU/XFX RX5700 XT THICC II Ultra OC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61786901-A3BD-4781-81D9-26BAFD6298C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDABB157-636C-45B2-84E0-5303B5DDA78F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="4290" windowWidth="28800" windowHeight="15435" xr2:uid="{70CB170A-B5BE-5B4E-9712-0A7B62ED3DB8}"/>
+    <workbookView xWindow="6435" yWindow="4005" windowWidth="28800" windowHeight="15435" xr2:uid="{70CB170A-B5BE-5B4E-9712-0A7B62ED3DB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1767,11 +1767,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="vanilla5700XT_1" growShrinkType="overwriteClear" connectionId="2" xr16:uid="{483F14D9-7952-D44F-94A2-CA8358672626}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="vanilla5700XT" growShrinkType="overwriteClear" connectionId="1" xr16:uid="{5FDEE6C4-83CF-A44B-9668-6DC544AB78C4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="vanilla5700XT" growShrinkType="overwriteClear" connectionId="1" xr16:uid="{5FDEE6C4-83CF-A44B-9668-6DC544AB78C4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="vanilla5700XT_1" growShrinkType="overwriteClear" connectionId="2" xr16:uid="{483F14D9-7952-D44F-94A2-CA8358672626}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2074,8 +2074,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:BG69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H68" sqref="H68:Y68"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB33" sqref="AB33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -4065,11 +4065,11 @@
       </c>
       <c r="T16" s="69" t="str">
         <f>AD37</f>
-        <v>4C</v>
+        <v>F4</v>
       </c>
       <c r="U16" s="70" t="str">
         <f>AE37</f>
-        <v>04</v>
+        <v>01</v>
       </c>
       <c r="V16" s="4" t="s">
         <v>4</v>
@@ -4079,11 +4079,11 @@
       </c>
       <c r="X16" s="69" t="str">
         <f>AD38</f>
-        <v>4C</v>
+        <v>F4</v>
       </c>
       <c r="Y16" s="72" t="str">
         <f>AE38</f>
-        <v>04</v>
+        <v>01</v>
       </c>
       <c r="Z16" s="4"/>
       <c r="AA16" s="20" t="s">
@@ -5340,15 +5340,15 @@
         <v>86</v>
       </c>
       <c r="AB26" s="39">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="AC26" s="39" t="str">
         <f>DEC2HEX(AB26,4)</f>
-        <v>0014</v>
+        <v>000F</v>
       </c>
       <c r="AD26" s="39" t="str">
         <f>MID(AC26,3,2)</f>
-        <v>14</v>
+        <v>0F</v>
       </c>
       <c r="AE26" s="39" t="str">
         <f>MID(AC26,1,2)</f>
@@ -6726,19 +6726,19 @@
         <v>94</v>
       </c>
       <c r="AB37" s="54">
-        <v>1100</v>
+        <v>500</v>
       </c>
       <c r="AC37" s="54" t="str">
         <f>DEC2HEX(AB37,4)</f>
-        <v>044C</v>
+        <v>01F4</v>
       </c>
       <c r="AD37" s="54" t="str">
         <f>MID(AC37,3,2)</f>
-        <v>4C</v>
+        <v>F4</v>
       </c>
       <c r="AE37" s="54" t="str">
         <f>MID(AC37,1,2)</f>
-        <v>04</v>
+        <v>01</v>
       </c>
       <c r="AF37" s="54"/>
       <c r="AG37" s="55" t="s">
@@ -6852,19 +6852,19 @@
         <v>95</v>
       </c>
       <c r="AB38" s="54">
-        <v>1100</v>
+        <v>500</v>
       </c>
       <c r="AC38" s="54" t="str">
         <f>DEC2HEX(AB38,4)</f>
-        <v>044C</v>
+        <v>01F4</v>
       </c>
       <c r="AD38" s="54" t="str">
         <f>MID(AC38,3,2)</f>
-        <v>4C</v>
+        <v>F4</v>
       </c>
       <c r="AE38" s="54" t="str">
         <f>MID(AC38,1,2)</f>
-        <v>04</v>
+        <v>01</v>
       </c>
       <c r="AF38" s="54"/>
       <c r="AG38" s="55" t="s">
@@ -7809,7 +7809,7 @@
       </c>
       <c r="R46" s="84" t="str">
         <f>AD26</f>
-        <v>14</v>
+        <v>0F</v>
       </c>
       <c r="S46" s="85" t="str">
         <f>AE26</f>
@@ -10279,7 +10279,7 @@
       <c r="G68" s="114"/>
       <c r="H68" s="115" t="str">
         <f>A1&amp;B1&amp;C1&amp;D1&amp;E1&amp;F1&amp;G1&amp;H1&amp;I1&amp;J1&amp;K1&amp;L1&amp;M1&amp;N1&amp;O1&amp;P1&amp;Q1&amp;R1&amp;S1&amp;T1&amp;U1&amp;V1&amp;W1&amp;X1&amp;Y1&amp;A2&amp;B2&amp;C2&amp;D2&amp;E2&amp;F2&amp;G2&amp;H2&amp;I2&amp;J2&amp;K2&amp;L2&amp;M2&amp;N2&amp;O2&amp;P2&amp;Q2&amp;R2&amp;S2&amp;T2&amp;U2&amp;V2&amp;W2&amp;X2&amp;Y2&amp;A3&amp;B3&amp;C3&amp;D3&amp;E3&amp;F3&amp;G3&amp;H3&amp;I3&amp;J3&amp;K3&amp;L3&amp;M3&amp;N3&amp;O3&amp;P3&amp;Q3&amp;R3&amp;S3&amp;T3&amp;U3&amp;V3&amp;W3&amp;X3&amp;Y3&amp;A4&amp;B4&amp;C4&amp;D4&amp;E4&amp;F4&amp;G4&amp;H4&amp;I4&amp;J4&amp;K4&amp;L4&amp;M4&amp;N4&amp;O4&amp;P4&amp;Q4&amp;R4&amp;S4&amp;T4&amp;U4&amp;V4&amp;W4&amp;X4&amp;Y4&amp;A5&amp;B5&amp;C5&amp;D5&amp;E5&amp;F5&amp;G5&amp;H5&amp;I5&amp;J5&amp;K5&amp;L5&amp;M5&amp;N5&amp;O5&amp;P5&amp;Q5&amp;R5&amp;S5&amp;T5&amp;U5&amp;V5&amp;W5&amp;X5&amp;Y5&amp;A6&amp;B6&amp;C6&amp;D6&amp;E6&amp;F6&amp;G6&amp;H6&amp;I6&amp;J6&amp;K6&amp;L6&amp;M6&amp;N6&amp;O6&amp;P6&amp;Q6&amp;R6&amp;S6&amp;T6&amp;U6&amp;V6&amp;W6&amp;X6&amp;Y6&amp;A7&amp;B7&amp;C7&amp;D7&amp;E7&amp;F7&amp;G7&amp;H7&amp;I7&amp;J7&amp;K7&amp;L7&amp;M7&amp;N7&amp;O7&amp;P7&amp;Q7&amp;R7&amp;S7&amp;T7&amp;U7&amp;V7&amp;W7&amp;X7&amp;Y7&amp;A8&amp;B8&amp;C8&amp;D8&amp;E8&amp;F8&amp;G8&amp;H8&amp;I8&amp;J8&amp;K8&amp;L8&amp;M8&amp;N8&amp;O8&amp;P8&amp;Q8&amp;R8&amp;S8&amp;T8&amp;U8&amp;V8&amp;W8&amp;X8&amp;Y8&amp;A9&amp;B9&amp;C9&amp;D9&amp;E9&amp;F9&amp;G9&amp;H9&amp;I9&amp;J9&amp;K9&amp;L9&amp;M9&amp;N9&amp;O9&amp;P9&amp;Q9&amp;R9&amp;S9&amp;T9&amp;U9&amp;V9&amp;W9&amp;X9&amp;Y9&amp;A10&amp;B10&amp;C10&amp;D10&amp;E10&amp;F10&amp;G10&amp;H10&amp;I10&amp;J10&amp;K10&amp;L10&amp;M10&amp;N10&amp;O10&amp;P10&amp;Q10&amp;R10&amp;S10&amp;T10&amp;U10&amp;V10&amp;W10&amp;X10&amp;Y10&amp;A11&amp;B11&amp;C11&amp;D11&amp;E11&amp;F11&amp;G11&amp;H11&amp;I11&amp;J11&amp;K11&amp;L11&amp;M11&amp;N11&amp;O11&amp;P11&amp;Q11&amp;R11&amp;S11&amp;T11&amp;U11&amp;V11&amp;W11&amp;X11&amp;Y11&amp;A12&amp;B12&amp;C12&amp;D12&amp;E12&amp;F12&amp;G12&amp;H12&amp;I12&amp;J12&amp;K12&amp;L12&amp;M12&amp;N12&amp;O12&amp;P12&amp;Q12&amp;R12&amp;S12&amp;T12&amp;U12&amp;V12&amp;W12&amp;X12&amp;Y12&amp;A13&amp;B13&amp;C13&amp;D13&amp;E13&amp;F13&amp;G13&amp;H13&amp;I13&amp;J13&amp;K13&amp;L13&amp;M13&amp;N13&amp;O13&amp;P13&amp;Q13&amp;R13&amp;S13&amp;T13&amp;U13&amp;V13&amp;W13&amp;X13&amp;Y13&amp;A14&amp;B14&amp;C14&amp;D14&amp;E14&amp;F14&amp;G14&amp;H14&amp;I14&amp;J14&amp;K14&amp;L14&amp;M14&amp;N14&amp;O14&amp;P14&amp;Q14&amp;R14&amp;S14&amp;T14&amp;U14&amp;V14&amp;W14&amp;X14&amp;Y14&amp;A15&amp;B15&amp;C15&amp;D15&amp;E15&amp;F15&amp;G15&amp;H15&amp;I15&amp;J15&amp;K15&amp;L15&amp;M15&amp;N15&amp;O15&amp;P15&amp;Q15&amp;R15&amp;S15&amp;T15&amp;U15&amp;V15&amp;W15&amp;X15&amp;Y15&amp;A16&amp;B16&amp;C16&amp;D16&amp;E16&amp;F16&amp;G16&amp;H16&amp;I16&amp;J16&amp;K16&amp;L16&amp;M16&amp;N16&amp;O16&amp;P16&amp;Q16&amp;R16&amp;S16&amp;T16&amp;U16&amp;V16&amp;W16&amp;X16&amp;Y16&amp;A17&amp;B17&amp;C17&amp;D17&amp;E17&amp;F17&amp;G17&amp;H17&amp;I17&amp;J17&amp;K17&amp;L17&amp;M17&amp;N17&amp;O17&amp;P17&amp;Q17&amp;R17&amp;S17&amp;T17&amp;U17&amp;V17&amp;W17&amp;X17&amp;Y17&amp;A18&amp;B18&amp;C18&amp;D18&amp;E18&amp;F18&amp;G18&amp;H18&amp;I18&amp;J18&amp;K18&amp;L18&amp;M18&amp;N18&amp;O18&amp;P18&amp;Q18&amp;R18&amp;S18&amp;T18&amp;U18&amp;V18&amp;W18&amp;X18&amp;Y18&amp;A19&amp;B19&amp;C19&amp;D19&amp;E19&amp;F19&amp;G19&amp;H19&amp;I19&amp;J19&amp;K19&amp;L19&amp;M19&amp;N19&amp;O19&amp;P19&amp;Q19&amp;R19&amp;S19&amp;T19&amp;U19&amp;V19&amp;W19&amp;X19&amp;Y19&amp;A20&amp;B20&amp;C20&amp;D20&amp;E20&amp;F20&amp;G20&amp;H20&amp;I20&amp;J20&amp;K20&amp;L20&amp;M20&amp;N20&amp;O20&amp;P20&amp;Q20&amp;R20&amp;S20&amp;T20&amp;U20&amp;V20&amp;W20&amp;X20&amp;Y20&amp;A21&amp;B21&amp;C21&amp;D21&amp;E21&amp;F21&amp;G21&amp;H21&amp;I21&amp;J21&amp;K21&amp;L21&amp;M21&amp;N21&amp;O21&amp;P21&amp;Q21&amp;R21&amp;S21&amp;T21&amp;U21&amp;V21&amp;W21&amp;X21&amp;Y21&amp;A22&amp;B22&amp;C22&amp;D22&amp;E22&amp;F22&amp;G22&amp;H22&amp;I22&amp;J22&amp;K22&amp;L22&amp;M22&amp;N22&amp;O22&amp;P22&amp;Q22&amp;R22&amp;S22&amp;T22&amp;U22&amp;V22&amp;W22&amp;X22&amp;Y22&amp;A23&amp;B23&amp;C23&amp;D23&amp;E23&amp;F23&amp;G23&amp;H23&amp;I23&amp;J23&amp;K23&amp;L23&amp;M23&amp;N23&amp;O23&amp;P23&amp;Q23&amp;R23&amp;S23&amp;T23&amp;U23&amp;V23&amp;W23&amp;X23&amp;Y23&amp;A24&amp;B24&amp;C24&amp;D24&amp;E24&amp;F24&amp;G24&amp;H24&amp;I24&amp;J24&amp;K24&amp;L24&amp;M24&amp;N24&amp;O24&amp;P24&amp;Q24&amp;R24&amp;S24&amp;T24&amp;U24&amp;V24&amp;W24&amp;X24&amp;Y24&amp;A25&amp;B25&amp;C25&amp;D25&amp;E25&amp;F25&amp;G25&amp;H25&amp;I25&amp;J25&amp;K25&amp;L25&amp;M25&amp;N25&amp;O25&amp;P25&amp;Q25&amp;R25&amp;S25&amp;T25&amp;U25&amp;V25&amp;W25&amp;X25&amp;Y25&amp;A26&amp;B26&amp;C26&amp;D26&amp;E26&amp;F26&amp;G26&amp;H26&amp;I26&amp;J26&amp;K26&amp;L26&amp;M26&amp;N26&amp;O26&amp;P26&amp;Q26&amp;R26&amp;S26&amp;T26&amp;U26&amp;V26&amp;W26&amp;X26&amp;Y26&amp;A27&amp;B27&amp;C27&amp;D27&amp;E27&amp;F27&amp;G27&amp;H27&amp;I27&amp;J27&amp;K27&amp;L27&amp;M27&amp;N27&amp;O27&amp;P27&amp;Q27&amp;R27&amp;S27&amp;T27&amp;U27&amp;V27&amp;W27&amp;X27&amp;Y27&amp;A28&amp;B28&amp;C28&amp;D28&amp;E28&amp;F28&amp;G28&amp;H28&amp;I28&amp;J28&amp;K28&amp;L28&amp;M28&amp;N28&amp;O28&amp;P28&amp;Q28&amp;R28&amp;S28&amp;T28&amp;U28&amp;V28&amp;W28&amp;X28&amp;Y28&amp;A29&amp;B29&amp;C29&amp;D29&amp;E29&amp;F29&amp;G29&amp;H29&amp;I29&amp;J29&amp;K29&amp;L29&amp;M29&amp;N29&amp;O29&amp;P29&amp;Q29&amp;R29&amp;S29&amp;T29&amp;U29&amp;V29&amp;W29&amp;X29&amp;Y29&amp;A30&amp;B30&amp;C30&amp;D30&amp;E30&amp;F30&amp;G30&amp;H30&amp;I30&amp;J30&amp;K30&amp;L30&amp;M30&amp;N30&amp;O30&amp;P30&amp;Q30&amp;R30&amp;S30&amp;T30&amp;U30&amp;V30&amp;W30&amp;X30&amp;Y30&amp;A31&amp;B31&amp;C31&amp;D31&amp;E31&amp;F31&amp;G31&amp;H31&amp;I31&amp;J31&amp;K31&amp;L31&amp;M31&amp;N31&amp;O31&amp;P31&amp;Q31&amp;R31&amp;S31&amp;T31&amp;U31&amp;V31&amp;W31&amp;X31&amp;Y31&amp;A32&amp;B32&amp;C32&amp;D32&amp;E32&amp;F32&amp;G32&amp;H32&amp;I32&amp;J32&amp;K32&amp;L32&amp;M32&amp;N32&amp;O32&amp;P32&amp;Q32&amp;R32&amp;S32&amp;T32&amp;U32&amp;V32&amp;W32&amp;X32&amp;Y32&amp;A33&amp;B33&amp;C33&amp;D33&amp;E33&amp;F33&amp;G33&amp;H33&amp;I33&amp;J33&amp;K33&amp;L33&amp;M33&amp;N33&amp;O33&amp;P33&amp;Q33&amp;R33&amp;S33&amp;T33&amp;U33&amp;V33&amp;W33&amp;X33&amp;Y33&amp;A34&amp;B34&amp;C34&amp;D34&amp;E34&amp;F34&amp;G34&amp;H34&amp;I34&amp;J34&amp;K34&amp;L34&amp;M34&amp;N34&amp;O34&amp;P34&amp;Q34&amp;R34&amp;S34&amp;T34&amp;U34&amp;V34&amp;W34&amp;X34&amp;Y34&amp;A35&amp;B35&amp;C35&amp;D35&amp;E35&amp;F35&amp;G35&amp;H35&amp;I35&amp;J35&amp;K35&amp;L35&amp;M35&amp;N35&amp;O35&amp;P35&amp;Q35&amp;R35&amp;S35&amp;T35&amp;U35&amp;V35&amp;W35&amp;X35&amp;Y35&amp;A36&amp;B36&amp;C36&amp;D36&amp;E36&amp;F36&amp;G36&amp;H36&amp;I36&amp;J36&amp;K36&amp;L36&amp;M36&amp;N36&amp;O36&amp;P36&amp;Q36&amp;R36&amp;S36&amp;T36&amp;U36&amp;V36&amp;W36&amp;X36&amp;Y36&amp;A37&amp;B37&amp;C37&amp;D37&amp;E37&amp;F37&amp;G37&amp;H37&amp;I37&amp;J37&amp;K37&amp;L37&amp;M37&amp;N37&amp;O37&amp;P37&amp;Q37&amp;R37&amp;S37&amp;T37&amp;U37&amp;V37&amp;W37&amp;X37&amp;Y37&amp;A38&amp;B38&amp;C38&amp;D38&amp;E38&amp;F38&amp;G38&amp;H38&amp;I38&amp;J38&amp;K38&amp;L38&amp;M38&amp;N38&amp;O38&amp;P38&amp;Q38&amp;R38&amp;S38&amp;T38&amp;U38&amp;V38&amp;W38&amp;X38&amp;Y38&amp;A39&amp;B39&amp;C39&amp;D39&amp;E39&amp;F39&amp;G39&amp;H39&amp;I39&amp;J39&amp;K39&amp;L39&amp;M39&amp;N39&amp;O39&amp;P39&amp;Q39&amp;R39&amp;S39&amp;T39&amp;U39&amp;V39&amp;W39&amp;X39&amp;Y39&amp;A40&amp;B40&amp;C40&amp;D40&amp;E40&amp;F40&amp;G40&amp;H40&amp;I40&amp;J40&amp;K40&amp;L40&amp;M40&amp;N40&amp;O40&amp;P40&amp;Q40&amp;R40&amp;S40&amp;T40&amp;U40&amp;V40&amp;W40&amp;X40&amp;Y40&amp;A41&amp;B41&amp;C41&amp;D41&amp;E41&amp;F41&amp;G41&amp;H41&amp;I41&amp;J41&amp;K41&amp;L41&amp;M41&amp;N41&amp;O41&amp;P41&amp;Q41&amp;R41&amp;S41&amp;T41&amp;U41&amp;V41&amp;W41&amp;X41&amp;Y41&amp;A42&amp;B42&amp;C42&amp;D42&amp;E42&amp;F42&amp;G42&amp;H42&amp;I42&amp;J42&amp;K42&amp;L42&amp;M42&amp;N42&amp;O42&amp;P42&amp;Q42&amp;R42&amp;S42&amp;T42&amp;U42&amp;V42&amp;W42&amp;X42&amp;Y42&amp;A43&amp;B43&amp;C43&amp;D43&amp;E43&amp;F43&amp;G43&amp;H43&amp;I43&amp;J43&amp;K43&amp;L43&amp;M43&amp;N43&amp;O43&amp;P43&amp;Q43&amp;R43&amp;S43&amp;T43&amp;U43&amp;V43&amp;W43&amp;X43&amp;Y43&amp;A44&amp;B44&amp;C44&amp;D44&amp;E44&amp;F44&amp;G44&amp;H44&amp;I44&amp;J44&amp;K44&amp;L44&amp;M44&amp;N44&amp;O44&amp;P44&amp;Q44&amp;R44&amp;S44&amp;T44&amp;U44&amp;V44&amp;W44&amp;X44&amp;Y44&amp;A45&amp;B45&amp;C45&amp;D45&amp;E45&amp;F45&amp;G45&amp;H45&amp;I45&amp;J45&amp;K45&amp;L45&amp;M45&amp;N45&amp;O45&amp;P45&amp;Q45&amp;R45&amp;S45&amp;T45&amp;U45&amp;V45&amp;W45&amp;X45&amp;Y45&amp;A46&amp;B46&amp;C46&amp;D46&amp;E46&amp;F46&amp;G46&amp;H46&amp;I46&amp;J46&amp;K46&amp;L46&amp;M46&amp;N46&amp;O46&amp;P46&amp;Q46&amp;R46&amp;S46&amp;T46&amp;U46&amp;V46&amp;W46&amp;X46&amp;Y46&amp;A47&amp;B47&amp;C47&amp;D47&amp;E47&amp;F47&amp;G47&amp;H47&amp;I47&amp;J47&amp;K47&amp;L47&amp;M47&amp;N47&amp;O47&amp;P47&amp;Q47&amp;R47&amp;S47&amp;T47&amp;U47&amp;V47&amp;W47&amp;X47&amp;Y47&amp;A48&amp;B48&amp;C48&amp;D48&amp;E48&amp;F48&amp;G48&amp;H48&amp;I48&amp;J48&amp;K48&amp;L48&amp;M48&amp;N48&amp;O48&amp;P48&amp;Q48&amp;R48&amp;S48&amp;T48&amp;U48&amp;V48&amp;W48&amp;X48&amp;Y48&amp;A49&amp;B49&amp;C49&amp;D49&amp;E49&amp;F49&amp;G49&amp;H49&amp;I49&amp;J49&amp;K49&amp;L49&amp;M49&amp;N49&amp;O49&amp;P49&amp;Q49&amp;R49&amp;S49&amp;T49&amp;U49&amp;V49&amp;W49&amp;X49&amp;Y49&amp;A50&amp;B50&amp;C50&amp;D50&amp;E50&amp;F50&amp;G50&amp;H50&amp;I50&amp;J50&amp;K50&amp;L50&amp;M50&amp;N50&amp;O50&amp;P50&amp;Q50&amp;R50&amp;S50&amp;T50&amp;U50&amp;V50&amp;W50&amp;X50&amp;Y50&amp;A51&amp;B51&amp;C51&amp;D51&amp;E51&amp;F51&amp;G51&amp;H51&amp;I51&amp;J51&amp;K51&amp;L51&amp;M51&amp;N51&amp;O51&amp;P51&amp;Q51&amp;R51&amp;S51&amp;T51&amp;U51&amp;V51&amp;W51&amp;X51&amp;Y51&amp;A52&amp;B52&amp;C52&amp;D52&amp;E52&amp;F52&amp;G52&amp;H52&amp;I52&amp;J52&amp;K52&amp;L52&amp;M52&amp;N52&amp;O52&amp;P52&amp;Q52&amp;R52&amp;S52&amp;T52&amp;U52&amp;V52&amp;W52&amp;X52&amp;Y52&amp;A53&amp;B53&amp;C53&amp;D53&amp;E53&amp;F53&amp;G53&amp;H53&amp;I53&amp;J53&amp;K53&amp;L53&amp;M53&amp;N53&amp;O53&amp;P53&amp;Q53&amp;R53&amp;S53&amp;T53&amp;U53&amp;V53&amp;W53&amp;X53&amp;Y53&amp;A54&amp;B54&amp;C54&amp;D54&amp;E54&amp;F54&amp;G54&amp;H54&amp;I54&amp;J54&amp;K54&amp;L54&amp;M54&amp;N54&amp;O54&amp;P54&amp;Q54&amp;R54&amp;S54&amp;T54&amp;U54&amp;V54&amp;W54&amp;X54&amp;Y54&amp;A55&amp;B55&amp;C55&amp;D55&amp;E55&amp;F55&amp;G55&amp;H55&amp;I55&amp;J55&amp;K55&amp;L55&amp;M55&amp;N55&amp;O55&amp;P55&amp;Q55&amp;R55&amp;S55&amp;T55&amp;U55&amp;V55&amp;W55&amp;X55&amp;Y55&amp;A56&amp;B56&amp;C56&amp;D56&amp;E56&amp;F56&amp;G56&amp;H56&amp;I56&amp;J56&amp;K56&amp;L56&amp;M56&amp;N56&amp;O56&amp;P56&amp;Q56&amp;R56&amp;S56&amp;T56&amp;U56&amp;V56&amp;W56&amp;X56&amp;Y56&amp;A57&amp;B57&amp;C57&amp;D57&amp;E57&amp;F57&amp;G57&amp;H57&amp;I57&amp;J57&amp;K57&amp;L57&amp;M57&amp;N57&amp;O57&amp;P57&amp;Q57&amp;R57&amp;S57&amp;T57&amp;U57&amp;V57&amp;W57&amp;X57&amp;Y57&amp;A58&amp;B58&amp;C58&amp;D58&amp;E58&amp;F58&amp;G58&amp;H58&amp;I58&amp;J58&amp;K58&amp;L58&amp;M58&amp;N58&amp;O58&amp;P58&amp;Q58&amp;R58&amp;S58&amp;T58&amp;U58&amp;V58&amp;W58&amp;X58&amp;Y58&amp;A59&amp;B59&amp;C59&amp;D59&amp;E59&amp;F59&amp;G59&amp;H59&amp;I59&amp;J59&amp;K59&amp;L59&amp;M59&amp;N59&amp;O59&amp;P59&amp;Q59&amp;R59&amp;S59&amp;T59&amp;U59&amp;V59&amp;W59&amp;X59&amp;Y59&amp;A60&amp;B60&amp;C60&amp;D60&amp;E60&amp;F60&amp;G60&amp;H60&amp;I60&amp;J60&amp;K60&amp;L60&amp;M60&amp;N60&amp;O60&amp;P60&amp;Q60&amp;R60&amp;S60&amp;T60&amp;U60&amp;V60&amp;W60&amp;X60&amp;Y60&amp;A61&amp;B61&amp;C61&amp;D61&amp;E61&amp;F61&amp;G61&amp;H61&amp;I61&amp;J61&amp;K61&amp;L61&amp;M61&amp;N61&amp;O61&amp;P61&amp;Q61&amp;R61&amp;S61&amp;T61&amp;U61&amp;V61&amp;W61&amp;X61&amp;Y61&amp;A62&amp;B62&amp;C62&amp;D62&amp;E62&amp;F62&amp;G62&amp;H62&amp;I62&amp;J62&amp;K62&amp;L62&amp;M62&amp;N62&amp;O62&amp;P62&amp;Q62&amp;R62&amp;S62&amp;T62&amp;U62&amp;V62&amp;W62&amp;X62&amp;Y62&amp;A63&amp;B63&amp;C63&amp;D63&amp;E63&amp;F63&amp;G63&amp;H63&amp;I63&amp;J63&amp;K63&amp;L63&amp;M63&amp;N63&amp;O63&amp;P63&amp;Q63&amp;R63&amp;S63&amp;T63&amp;U63&amp;V63&amp;W63&amp;X63&amp;Y63&amp;A64&amp;B64&amp;C64&amp;D64&amp;E64&amp;F64&amp;G64&amp;H64&amp;I64&amp;J64&amp;K64&amp;L64&amp;M64&amp;N64&amp;O64&amp;P64&amp;Q64&amp;R64&amp;S64&amp;T64&amp;U64&amp;V64&amp;W64&amp;X64&amp;Y64&amp;A65&amp;B65&amp;C65&amp;D65&amp;E65&amp;F65&amp;G65&amp;H65&amp;I65&amp;J65&amp;K65&amp;L65&amp;M65&amp;N65&amp;O65&amp;P65&amp;Q65&amp;R65&amp;S65&amp;T65&amp;U65&amp;V65&amp;W65&amp;X65&amp;Y65&amp;A66&amp;B66&amp;C66&amp;D66&amp;E66&amp;F66&amp;G66&amp;H66&amp;I66&amp;J66&amp;K66&amp;L66&amp;M66&amp;N66&amp;O66&amp;P66&amp;Q66&amp;R66&amp;S66&amp;T66&amp;U66&amp;V66&amp;W66&amp;X66&amp;Y66&amp;A67&amp;B67&amp;C67&amp;D67&amp;E67&amp;F67&amp;G67&amp;H67&amp;I67&amp;J67&amp;K67&amp;L67&amp;M67&amp;N67&amp;O67&amp;P67&amp;Q67&amp;R67&amp;S67&amp;T67&amp;U67&amp;V67&amp;W67&amp;X67</f>
-        <v>8A060C0001E201C7080000203800007D00080000001B000000000000000000007600000000000000000000000000010000000A00000034080000F30400003E040000F3040000F30400006B030000F304000004050000040500002A0300000000000000000000000000000000000000000000000000002C010000640000006400000064000000FB01000064000000FB010000340100002C0100002C010000000000000000000000000000000000000000000000000000800000000E0000001E0000000101010101010101010001010101000000000000000000000000000000000000980800009808000098080000B004000098080000B004000098080000B0040000B603000032000000AC0D0000AC0D0000640000006E000000020000000100000001000000010000000100000064000000640000006400000064000000640000006400000064000000640000006400000064000000000000000000000000000000200300002003000020030000EE02000020030000EE02000020030000EE02000071020000320000004C0400004C04000019000000320000000000000000000000000000000000000000000000190000000A000000190000000A000000190000000A000000190000000A000000190000000A00000000000000000000000000000008000000FFAFDFB323060000D2000000000000000000000000000000D20000000000000000000000000000000E000000C400000064006E00690073007300730073000000000000000000000000000000FE70000001000000640064000000000000000000540B540BB80BB80BC01268104C0000000100020000000000000000008126823EA4705DBEB51A323F010002000000803F00000000F1BA5E3EABB26FBD45F5363F010104000000803F00000000F1BA5E3EABB26FBD45F5363F01000200D8F0243F35EF083F00000000D42BC53E575B113F010002000A68023F14AE173F000000008351A93E3789113F010002009CC4A03F8E06B0BE00000000E3C7083FEC2F7B3E010002006154523FD7346F3C00000000FD87F43ECA54813E0200020000000000000000000000000000000000000000000200020000000000000000000000000000000000000000002C016608780578057805780578057805780578057805780578057805780578056400F304F304F304F304F304F304F30464003E043E043E043E043E043E043E04FB01F304B603B603B603B603B603B6036400F4017102B603FB01F304F304F304F304F304F304F304340104050405040504050405040504052C010405A404A404A404A404A404A4042C012A032A032A032A032A032A032A03D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D0013408F3046B033E04F304F304040504052A03D001000303033001FB01B80BB80B8C0A480D480D480D881318151815181520032003200300000000D0010000010200005B0000100000000306066B026B0200000000000000002D003700900190019001900190019001900190019001900114004006AC0DAC0D590020030100010200000000000000000000000047E6913CACA841BD13445D3D00000000000000008FC2F53C0000000000000000000000004BC8C73D9834463D7042A1BDAF5A193B8CA11CBBF836BD3D00000000000000000000000000000000000000000000000000000000000000000000000000000000A000A0000101000000000000A000A0000002000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000A901870087000000000000000000000000000000190019000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>8A060C0001E201C7080000203800007D00080000001B000000000000000000007600000000000000000000000000010000000A00000034080000F30400003E040000F3040000F30400006B030000F304000004050000040500002A0300000000000000000000000000000000000000000000000000002C010000640000006400000064000000FB01000064000000FB010000340100002C0100002C010000000000000000000000000000000000000000000000000000800000000E0000001E0000000101010101010101010001010101000000000000000000000000000000000000980800009808000098080000B004000098080000B004000098080000B0040000B603000032000000AC0D0000AC0D0000640000006E000000020000000100000001000000010000000100000064000000640000006400000064000000640000006400000064000000640000006400000064000000000000000000000000000000200300002003000020030000EE02000020030000EE02000020030000EE0200007102000032000000F4010000F401000019000000320000000000000000000000000000000000000000000000190000000A000000190000000A000000190000000A000000190000000A000000190000000A00000000000000000000000000000008000000FFAFDFB323060000D2000000000000000000000000000000D20000000000000000000000000000000E000000C400000064006E00690073007300730073000000000000000000000000000000FE70000001000000640064000000000000000000540B540BB80BB80BC01268104C0000000100020000000000000000008126823EA4705DBEB51A323F010002000000803F00000000F1BA5E3EABB26FBD45F5363F010104000000803F00000000F1BA5E3EABB26FBD45F5363F01000200D8F0243F35EF083F00000000D42BC53E575B113F010002000A68023F14AE173F000000008351A93E3789113F010002009CC4A03F8E06B0BE00000000E3C7083FEC2F7B3E010002006154523FD7346F3C00000000FD87F43ECA54813E0200020000000000000000000000000000000000000000000200020000000000000000000000000000000000000000002C016608780578057805780578057805780578057805780578057805780578056400F304F304F304F304F304F304F30464003E043E043E043E043E043E043E04FB01F304B603B603B603B603B603B6036400F4017102B603FB01F304F304F304F304F304F304F304340104050405040504050405040504052C010405A404A404A404A404A404A4042C012A032A032A032A032A032A032A03D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D001D0013408F3046B033E04F304F304040504052A03D001000303033001FB01B80BB80B8C0A480D480D480D881318151815181520032003200300000000D0010000010200005B0000100000000306066B026B0200000000000000002D00370090019001900190019001900190019001900190010F004006AC0DAC0D590020030100010200000000000000000000000047E6913CACA841BD13445D3D00000000000000008FC2F53C0000000000000000000000004BC8C73D9834463D7042A1BDAF5A193B8CA11CBBF836BD3D00000000000000000000000000000000000000000000000000000000000000000000000000000000A000A0000101000000000000A000A0000002000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000A901870087000000000000000000000000000000190019000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="I68" s="116"/>
       <c r="J68" s="116"/>

</xml_diff>